<commit_message>
expanded column key support
</commit_message>
<xml_diff>
--- a/test/fixtures/custom_check/sample.xlsx
+++ b/test/fixtures/custom_check/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="MainData"/>
@@ -115,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,12 +156,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -228,14 +222,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,16 +532,16 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="6.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="6.719285714285714" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="25.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="9.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="17.433571428571426" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="19.005" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
@@ -561,8 +552,8 @@
     <col min="12" max="12" style="5" width="25.14785714285714" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="5" width="29.862142857142857" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="5" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="15" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="15" width="29.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="14" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="14" width="29.862142857142857" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="5" width="12.719285714285713" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="15.43357142857143" customWidth="1" bestFit="1"/>
@@ -854,8 +845,8 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -892,8 +883,8 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -930,8 +921,8 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -965,7 +956,7 @@
   </sheetPr>
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -1033,7 +1024,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1066,7 +1057,7 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1095,7 +1086,7 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1124,7 +1115,7 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1153,7 +1144,7 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1182,7 +1173,7 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1211,7 +1202,7 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1240,7 +1231,7 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>

</xml_diff>